<commit_message>
cap nhat importexcel taisan/vitri, fix dm loai bao tri, ke hoach bao tri
</commit_message>
<xml_diff>
--- a/web/uploads/excel/down/mau_import_he_thong.xlsx
+++ b/web/uploads/excel/down/mau_import_he_thong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Disk\wamp64\www\qlts\web\uploads\excel\down\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\qlts\web\uploads\excel\down\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2AC582-7689-4F1F-A7C2-27C5C40986B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28D6E7F-FE4E-43DA-A4BD-BDC14E1863D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>STT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Mô tả/Ghi chú</t>
@@ -185,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,27 +214,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,176 +506,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="21"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="G2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="G4"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
+      <c r="G5"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
+      <c r="G6"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
+      <c r="G7"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>